<commit_message>
popisy jsou důležitý... I guess
</commit_message>
<xml_diff>
--- a/Dummymappe2csv.xlsx
+++ b/Dummymappe2csv.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Firma</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Pan les</t>
+  </si>
+  <si>
+    <t>ano</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,6 +596,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Input of the name
</commit_message>
<xml_diff>
--- a/Dummymappe2csv.xlsx
+++ b/Dummymappe2csv.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>